<commit_message>
removed test and general cleanup
</commit_message>
<xml_diff>
--- a/Name.xlsx
+++ b/Name.xlsx
@@ -460,10 +460,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4.53</v>
+        <v>4.45</v>
       </c>
       <c r="C12" t="n">
-        <v>7.13</v>
+        <v>6.47</v>
       </c>
     </row>
     <row r="13">
@@ -473,10 +473,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4.71</v>
+        <v>4.63</v>
       </c>
       <c r="C13" t="n">
-        <v>11.22</v>
+        <v>10.53</v>
       </c>
     </row>
     <row r="14">
@@ -486,10 +486,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.33</v>
+        <v>-0.41</v>
       </c>
       <c r="C14" t="n">
-        <v>8.27</v>
+        <v>7.61</v>
       </c>
     </row>
     <row r="15">
@@ -499,10 +499,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4.71</v>
+        <v>4.63</v>
       </c>
       <c r="C15" t="n">
-        <v>11.22</v>
+        <v>10.53</v>
       </c>
     </row>
     <row r="16">
@@ -575,10 +575,10 @@
         <v>44943</v>
       </c>
       <c r="B21" t="n">
-        <v>136.0498962402344</v>
+        <v>135.9400024414062</v>
       </c>
       <c r="C21" t="n">
-        <v>72.03500366210938</v>
+        <v>71.58999633789062</v>
       </c>
     </row>
     <row r="22">

</xml_diff>